<commit_message>
Improvements in the mechanism dealing with computation of the statistics based on the exam results.
</commit_message>
<xml_diff>
--- a/inst/as_egzaminy.xlsx
+++ b/inst/as_egzaminy.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zajac/Dropbox/PEJK/ASIA/dane do testowania/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zajac/Dropbox/PEJK/ASIA/Pakiet ASIA/ASIA1/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB4F434-46EF-8642-B428-55FC7E689154}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FAC9F6-D228-8544-B9C8-D5F92BB1A89B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="5160" windowWidth="21900" windowHeight="15300" xr2:uid="{426D8DBF-BA16-D948-8B32-547E5522B24E}"/>
+    <workbookView xWindow="12440" yWindow="5200" windowWidth="24300" windowHeight="15360" xr2:uid="{426D8DBF-BA16-D948-8B32-547E5522B24E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="15">
   <si>
     <t>pesel</t>
   </si>
@@ -422,15 +422,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26715E4D-2C3A-A745-9ED6-AD0EA8355743}">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103:J120"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -467,7 +468,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>97040200001</v>
+        <v>98090100001</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -497,7 +498,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>97040200002</v>
+        <v>98090100002</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -527,7 +528,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>97040200003</v>
+        <v>98090100003</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -557,7 +558,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>97040200004</v>
+        <v>98090100004</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -587,7 +588,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>97040200005</v>
+        <v>98090100005</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -617,7 +618,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>97040200006</v>
+        <v>98090100006</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -647,7 +648,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>97040200007</v>
+        <v>98090100007</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -677,7 +678,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>97040200008</v>
+        <v>98090100008</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -707,7 +708,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>97040200009</v>
+        <v>98090100009</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -737,7 +738,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>97040200010</v>
+        <v>98090100010</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -767,7 +768,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>97040200011</v>
+        <v>98090100011</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -797,7 +798,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>97040200012</v>
+        <v>98090100012</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -827,7 +828,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>97040200013</v>
+        <v>98090100013</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -857,7 +858,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>97040200014</v>
+        <v>98090100014</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -887,7 +888,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>97040200015</v>
+        <v>98090100015</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -917,7 +918,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>97040200016</v>
+        <v>98090100016</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -947,7 +948,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>97040200017</v>
+        <v>98090100017</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -977,7 +978,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>97040200018</v>
+        <v>98090100018</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
@@ -1007,7 +1008,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>97040200019</v>
+        <v>98090100019</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -1037,7 +1038,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>97040200020</v>
+        <v>98090100020</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -1067,7 +1068,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>97040200021</v>
+        <v>98090100021</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -1097,7 +1098,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>97040200022</v>
+        <v>98090100022</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
@@ -1127,7 +1128,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>97040200023</v>
+        <v>98090100023</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
@@ -1157,7 +1158,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>97040200024</v>
+        <v>98090100024</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
@@ -1187,7 +1188,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>97040200025</v>
+        <v>98090100025</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
@@ -1217,7 +1218,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>97040200026</v>
+        <v>98090100026</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -1247,7 +1248,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>97040200027</v>
+        <v>98090100027</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
@@ -1277,7 +1278,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>97040200028</v>
+        <v>98090100028</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -1307,7 +1308,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>97040200029</v>
+        <v>98090100029</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -1337,7 +1338,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>97040200030</v>
+        <v>98090100030</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -1367,7 +1368,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>97040200001</v>
+        <v>98090100001</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
@@ -1397,7 +1398,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>97040200002</v>
+        <v>98090100002</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
@@ -1427,7 +1428,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>97040200003</v>
+        <v>98090100003</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
@@ -1457,7 +1458,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>97040200004</v>
+        <v>98090100004</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
@@ -1487,7 +1488,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>97040200005</v>
+        <v>98090100005</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
@@ -1517,7 +1518,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>97040200006</v>
+        <v>98090100006</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
@@ -1547,7 +1548,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>97040200007</v>
+        <v>98090100007</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
@@ -1577,7 +1578,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>97040200008</v>
+        <v>98090100008</v>
       </c>
       <c r="B39" t="s">
         <v>12</v>
@@ -1607,7 +1608,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>97040200009</v>
+        <v>98090100009</v>
       </c>
       <c r="B40" t="s">
         <v>12</v>
@@ -1637,7 +1638,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>97040200010</v>
+        <v>98090100010</v>
       </c>
       <c r="B41" t="s">
         <v>12</v>
@@ -1667,7 +1668,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>97040200011</v>
+        <v>98090100011</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
@@ -1697,7 +1698,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>97040200012</v>
+        <v>98090100012</v>
       </c>
       <c r="B43" t="s">
         <v>12</v>
@@ -1727,7 +1728,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>97040200013</v>
+        <v>98090100013</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
@@ -1757,7 +1758,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>97040200014</v>
+        <v>98090100014</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
@@ -1787,7 +1788,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>97040200015</v>
+        <v>98090100015</v>
       </c>
       <c r="B46" t="s">
         <v>12</v>
@@ -1817,7 +1818,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>97040200016</v>
+        <v>98090100016</v>
       </c>
       <c r="B47" t="s">
         <v>12</v>
@@ -1847,7 +1848,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>97040200017</v>
+        <v>98090100017</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
@@ -1877,7 +1878,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>97040200018</v>
+        <v>98090100018</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
@@ -1907,7 +1908,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>97040200019</v>
+        <v>98090100019</v>
       </c>
       <c r="B50" t="s">
         <v>12</v>
@@ -1937,7 +1938,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>97040200020</v>
+        <v>98090100020</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
@@ -1967,7 +1968,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>97040200021</v>
+        <v>98090100021</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
@@ -1997,7 +1998,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>97040200022</v>
+        <v>98090100022</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
@@ -2027,7 +2028,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>97040200023</v>
+        <v>98090100023</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
@@ -2057,7 +2058,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>97040200024</v>
+        <v>98090100024</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
@@ -2087,7 +2088,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>97040200025</v>
+        <v>98090100025</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
@@ -2117,7 +2118,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>97040200026</v>
+        <v>98090100026</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
@@ -2147,7 +2148,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>97040200027</v>
+        <v>98090100027</v>
       </c>
       <c r="B58" t="s">
         <v>12</v>
@@ -2177,7 +2178,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>97040200028</v>
+        <v>98090100028</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
@@ -2207,7 +2208,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>97040200029</v>
+        <v>98090100029</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
@@ -2237,7 +2238,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>97040200030</v>
+        <v>98090100030</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
@@ -3882,6 +3883,906 @@
         <v>10</v>
       </c>
       <c r="J120">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>98090100001</v>
+      </c>
+      <c r="B121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D121">
+        <f>E121+F121</f>
+        <v>200</v>
+      </c>
+      <c r="E121">
+        <v>100</v>
+      </c>
+      <c r="F121">
+        <v>100</v>
+      </c>
+      <c r="G121" t="s">
+        <v>10</v>
+      </c>
+      <c r="H121" t="s">
+        <v>10</v>
+      </c>
+      <c r="I121" t="s">
+        <v>10</v>
+      </c>
+      <c r="J121">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>98090100002</v>
+      </c>
+      <c r="B122" t="s">
+        <v>14</v>
+      </c>
+      <c r="D122">
+        <f t="shared" ref="D122:D150" si="3">E122+F122</f>
+        <v>198</v>
+      </c>
+      <c r="E122">
+        <v>99</v>
+      </c>
+      <c r="F122">
+        <v>99</v>
+      </c>
+      <c r="G122" t="s">
+        <v>10</v>
+      </c>
+      <c r="H122" t="s">
+        <v>10</v>
+      </c>
+      <c r="I122" t="s">
+        <v>10</v>
+      </c>
+      <c r="J122">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>98090100003</v>
+      </c>
+      <c r="B123" t="s">
+        <v>14</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="3"/>
+        <v>196</v>
+      </c>
+      <c r="E123">
+        <v>98</v>
+      </c>
+      <c r="F123">
+        <v>98</v>
+      </c>
+      <c r="G123" t="s">
+        <v>10</v>
+      </c>
+      <c r="H123" t="s">
+        <v>10</v>
+      </c>
+      <c r="I123" t="s">
+        <v>10</v>
+      </c>
+      <c r="J123">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>98090100004</v>
+      </c>
+      <c r="B124" t="s">
+        <v>14</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="3"/>
+        <v>194</v>
+      </c>
+      <c r="E124">
+        <v>97</v>
+      </c>
+      <c r="F124">
+        <v>97</v>
+      </c>
+      <c r="G124" t="s">
+        <v>10</v>
+      </c>
+      <c r="H124" t="s">
+        <v>10</v>
+      </c>
+      <c r="I124" t="s">
+        <v>10</v>
+      </c>
+      <c r="J124">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>98090100005</v>
+      </c>
+      <c r="B125" t="s">
+        <v>14</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="3"/>
+        <v>192</v>
+      </c>
+      <c r="E125">
+        <v>96</v>
+      </c>
+      <c r="F125">
+        <v>96</v>
+      </c>
+      <c r="G125" t="s">
+        <v>10</v>
+      </c>
+      <c r="H125" t="s">
+        <v>10</v>
+      </c>
+      <c r="I125" t="s">
+        <v>10</v>
+      </c>
+      <c r="J125">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>98090100006</v>
+      </c>
+      <c r="B126" t="s">
+        <v>14</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="3"/>
+        <v>190</v>
+      </c>
+      <c r="E126">
+        <v>95</v>
+      </c>
+      <c r="F126">
+        <v>95</v>
+      </c>
+      <c r="G126" t="s">
+        <v>10</v>
+      </c>
+      <c r="H126" t="s">
+        <v>10</v>
+      </c>
+      <c r="I126" t="s">
+        <v>10</v>
+      </c>
+      <c r="J126">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>98090100007</v>
+      </c>
+      <c r="B127" t="s">
+        <v>14</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="3"/>
+        <v>188</v>
+      </c>
+      <c r="E127">
+        <v>94</v>
+      </c>
+      <c r="F127">
+        <v>94</v>
+      </c>
+      <c r="G127" t="s">
+        <v>10</v>
+      </c>
+      <c r="H127" t="s">
+        <v>10</v>
+      </c>
+      <c r="I127" t="s">
+        <v>10</v>
+      </c>
+      <c r="J127">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>98090100008</v>
+      </c>
+      <c r="B128" t="s">
+        <v>14</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="3"/>
+        <v>186</v>
+      </c>
+      <c r="E128">
+        <v>93</v>
+      </c>
+      <c r="F128">
+        <v>93</v>
+      </c>
+      <c r="G128" t="s">
+        <v>10</v>
+      </c>
+      <c r="H128" t="s">
+        <v>10</v>
+      </c>
+      <c r="I128" t="s">
+        <v>10</v>
+      </c>
+      <c r="J128">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>98090100009</v>
+      </c>
+      <c r="B129" t="s">
+        <v>14</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="3"/>
+        <v>184</v>
+      </c>
+      <c r="E129">
+        <v>92</v>
+      </c>
+      <c r="F129">
+        <v>92</v>
+      </c>
+      <c r="G129" t="s">
+        <v>10</v>
+      </c>
+      <c r="H129" t="s">
+        <v>10</v>
+      </c>
+      <c r="I129" t="s">
+        <v>10</v>
+      </c>
+      <c r="J129">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>98090100010</v>
+      </c>
+      <c r="B130" t="s">
+        <v>14</v>
+      </c>
+      <c r="D130">
+        <f t="shared" si="3"/>
+        <v>182</v>
+      </c>
+      <c r="E130">
+        <v>91</v>
+      </c>
+      <c r="F130">
+        <v>91</v>
+      </c>
+      <c r="G130" t="s">
+        <v>10</v>
+      </c>
+      <c r="H130" t="s">
+        <v>10</v>
+      </c>
+      <c r="I130" t="s">
+        <v>10</v>
+      </c>
+      <c r="J130">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>98090100011</v>
+      </c>
+      <c r="B131" t="s">
+        <v>14</v>
+      </c>
+      <c r="D131">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+      <c r="E131">
+        <v>90</v>
+      </c>
+      <c r="F131">
+        <v>90</v>
+      </c>
+      <c r="G131" t="s">
+        <v>10</v>
+      </c>
+      <c r="H131" t="s">
+        <v>10</v>
+      </c>
+      <c r="I131" t="s">
+        <v>10</v>
+      </c>
+      <c r="J131">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>98090100012</v>
+      </c>
+      <c r="B132" t="s">
+        <v>14</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="3"/>
+        <v>178</v>
+      </c>
+      <c r="E132">
+        <v>89</v>
+      </c>
+      <c r="F132">
+        <v>89</v>
+      </c>
+      <c r="G132" t="s">
+        <v>10</v>
+      </c>
+      <c r="H132" t="s">
+        <v>10</v>
+      </c>
+      <c r="I132" t="s">
+        <v>10</v>
+      </c>
+      <c r="J132">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>98090100013</v>
+      </c>
+      <c r="B133" t="s">
+        <v>14</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="3"/>
+        <v>176</v>
+      </c>
+      <c r="E133">
+        <v>88</v>
+      </c>
+      <c r="F133">
+        <v>88</v>
+      </c>
+      <c r="G133" t="s">
+        <v>10</v>
+      </c>
+      <c r="H133" t="s">
+        <v>10</v>
+      </c>
+      <c r="I133" t="s">
+        <v>10</v>
+      </c>
+      <c r="J133">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>98090100014</v>
+      </c>
+      <c r="B134" t="s">
+        <v>14</v>
+      </c>
+      <c r="D134">
+        <f t="shared" si="3"/>
+        <v>174</v>
+      </c>
+      <c r="E134">
+        <v>87</v>
+      </c>
+      <c r="F134">
+        <v>87</v>
+      </c>
+      <c r="G134" t="s">
+        <v>10</v>
+      </c>
+      <c r="H134" t="s">
+        <v>10</v>
+      </c>
+      <c r="I134" t="s">
+        <v>10</v>
+      </c>
+      <c r="J134">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>98090100015</v>
+      </c>
+      <c r="B135" t="s">
+        <v>14</v>
+      </c>
+      <c r="D135">
+        <f t="shared" si="3"/>
+        <v>172</v>
+      </c>
+      <c r="E135">
+        <v>86</v>
+      </c>
+      <c r="F135">
+        <v>86</v>
+      </c>
+      <c r="G135" t="s">
+        <v>10</v>
+      </c>
+      <c r="H135" t="s">
+        <v>10</v>
+      </c>
+      <c r="I135" t="s">
+        <v>10</v>
+      </c>
+      <c r="J135">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>98090100016</v>
+      </c>
+      <c r="B136" t="s">
+        <v>14</v>
+      </c>
+      <c r="D136">
+        <f t="shared" si="3"/>
+        <v>170</v>
+      </c>
+      <c r="E136">
+        <v>85</v>
+      </c>
+      <c r="F136">
+        <v>85</v>
+      </c>
+      <c r="G136" t="s">
+        <v>10</v>
+      </c>
+      <c r="H136" t="s">
+        <v>10</v>
+      </c>
+      <c r="I136" t="s">
+        <v>10</v>
+      </c>
+      <c r="J136">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>98090100017</v>
+      </c>
+      <c r="B137" t="s">
+        <v>14</v>
+      </c>
+      <c r="D137">
+        <f t="shared" si="3"/>
+        <v>168</v>
+      </c>
+      <c r="E137">
+        <v>84</v>
+      </c>
+      <c r="F137">
+        <v>84</v>
+      </c>
+      <c r="G137" t="s">
+        <v>10</v>
+      </c>
+      <c r="H137" t="s">
+        <v>10</v>
+      </c>
+      <c r="I137" t="s">
+        <v>10</v>
+      </c>
+      <c r="J137">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>98090100018</v>
+      </c>
+      <c r="B138" t="s">
+        <v>14</v>
+      </c>
+      <c r="D138">
+        <f t="shared" si="3"/>
+        <v>166</v>
+      </c>
+      <c r="E138">
+        <v>83</v>
+      </c>
+      <c r="F138">
+        <v>83</v>
+      </c>
+      <c r="G138" t="s">
+        <v>10</v>
+      </c>
+      <c r="H138" t="s">
+        <v>10</v>
+      </c>
+      <c r="I138" t="s">
+        <v>10</v>
+      </c>
+      <c r="J138">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>98090100019</v>
+      </c>
+      <c r="B139" t="s">
+        <v>14</v>
+      </c>
+      <c r="D139">
+        <f t="shared" si="3"/>
+        <v>164</v>
+      </c>
+      <c r="E139">
+        <v>82</v>
+      </c>
+      <c r="F139">
+        <v>82</v>
+      </c>
+      <c r="G139" t="s">
+        <v>10</v>
+      </c>
+      <c r="H139" t="s">
+        <v>10</v>
+      </c>
+      <c r="I139" t="s">
+        <v>10</v>
+      </c>
+      <c r="J139">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>98090100020</v>
+      </c>
+      <c r="B140" t="s">
+        <v>14</v>
+      </c>
+      <c r="D140">
+        <f t="shared" si="3"/>
+        <v>162</v>
+      </c>
+      <c r="E140">
+        <v>81</v>
+      </c>
+      <c r="F140">
+        <v>81</v>
+      </c>
+      <c r="G140" t="s">
+        <v>10</v>
+      </c>
+      <c r="H140" t="s">
+        <v>10</v>
+      </c>
+      <c r="I140" t="s">
+        <v>10</v>
+      </c>
+      <c r="J140">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>98090100021</v>
+      </c>
+      <c r="B141" t="s">
+        <v>14</v>
+      </c>
+      <c r="D141">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+      <c r="E141">
+        <v>80</v>
+      </c>
+      <c r="F141">
+        <v>80</v>
+      </c>
+      <c r="G141" t="s">
+        <v>10</v>
+      </c>
+      <c r="H141" t="s">
+        <v>10</v>
+      </c>
+      <c r="I141" t="s">
+        <v>10</v>
+      </c>
+      <c r="J141">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>98090100022</v>
+      </c>
+      <c r="B142" t="s">
+        <v>14</v>
+      </c>
+      <c r="D142">
+        <f t="shared" si="3"/>
+        <v>158</v>
+      </c>
+      <c r="E142">
+        <v>79</v>
+      </c>
+      <c r="F142">
+        <v>79</v>
+      </c>
+      <c r="G142" t="s">
+        <v>10</v>
+      </c>
+      <c r="H142" t="s">
+        <v>10</v>
+      </c>
+      <c r="I142" t="s">
+        <v>10</v>
+      </c>
+      <c r="J142">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>98090100023</v>
+      </c>
+      <c r="B143" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143">
+        <f t="shared" si="3"/>
+        <v>156</v>
+      </c>
+      <c r="E143">
+        <v>78</v>
+      </c>
+      <c r="F143">
+        <v>78</v>
+      </c>
+      <c r="G143" t="s">
+        <v>10</v>
+      </c>
+      <c r="H143" t="s">
+        <v>10</v>
+      </c>
+      <c r="I143" t="s">
+        <v>10</v>
+      </c>
+      <c r="J143">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>98090100024</v>
+      </c>
+      <c r="B144" t="s">
+        <v>14</v>
+      </c>
+      <c r="D144">
+        <f t="shared" si="3"/>
+        <v>154</v>
+      </c>
+      <c r="E144">
+        <v>77</v>
+      </c>
+      <c r="F144">
+        <v>77</v>
+      </c>
+      <c r="G144" t="s">
+        <v>10</v>
+      </c>
+      <c r="H144" t="s">
+        <v>10</v>
+      </c>
+      <c r="I144" t="s">
+        <v>10</v>
+      </c>
+      <c r="J144">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>98090100025</v>
+      </c>
+      <c r="B145" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145">
+        <f t="shared" si="3"/>
+        <v>152</v>
+      </c>
+      <c r="E145">
+        <v>76</v>
+      </c>
+      <c r="F145">
+        <v>76</v>
+      </c>
+      <c r="G145" t="s">
+        <v>10</v>
+      </c>
+      <c r="H145" t="s">
+        <v>10</v>
+      </c>
+      <c r="I145" t="s">
+        <v>10</v>
+      </c>
+      <c r="J145">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>98090100026</v>
+      </c>
+      <c r="B146" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="E146">
+        <v>75</v>
+      </c>
+      <c r="F146">
+        <v>75</v>
+      </c>
+      <c r="G146" t="s">
+        <v>10</v>
+      </c>
+      <c r="H146" t="s">
+        <v>10</v>
+      </c>
+      <c r="I146" t="s">
+        <v>10</v>
+      </c>
+      <c r="J146">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>98090100027</v>
+      </c>
+      <c r="B147" t="s">
+        <v>14</v>
+      </c>
+      <c r="D147">
+        <f t="shared" si="3"/>
+        <v>148</v>
+      </c>
+      <c r="E147">
+        <v>74</v>
+      </c>
+      <c r="F147">
+        <v>74</v>
+      </c>
+      <c r="G147" t="s">
+        <v>10</v>
+      </c>
+      <c r="H147" t="s">
+        <v>10</v>
+      </c>
+      <c r="I147" t="s">
+        <v>10</v>
+      </c>
+      <c r="J147">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>98090100028</v>
+      </c>
+      <c r="B148" t="s">
+        <v>14</v>
+      </c>
+      <c r="D148">
+        <f t="shared" si="3"/>
+        <v>146</v>
+      </c>
+      <c r="E148">
+        <v>73</v>
+      </c>
+      <c r="F148">
+        <v>73</v>
+      </c>
+      <c r="G148" t="s">
+        <v>10</v>
+      </c>
+      <c r="H148" t="s">
+        <v>10</v>
+      </c>
+      <c r="I148" t="s">
+        <v>10</v>
+      </c>
+      <c r="J148">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>98090100029</v>
+      </c>
+      <c r="B149" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149">
+        <f t="shared" si="3"/>
+        <v>144</v>
+      </c>
+      <c r="E149">
+        <v>72</v>
+      </c>
+      <c r="F149">
+        <v>72</v>
+      </c>
+      <c r="G149" t="s">
+        <v>10</v>
+      </c>
+      <c r="H149" t="s">
+        <v>10</v>
+      </c>
+      <c r="I149" t="s">
+        <v>10</v>
+      </c>
+      <c r="J149">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>98090100030</v>
+      </c>
+      <c r="B150" t="s">
+        <v>14</v>
+      </c>
+      <c r="D150">
+        <f t="shared" si="3"/>
+        <v>142</v>
+      </c>
+      <c r="E150">
+        <v>71</v>
+      </c>
+      <c r="F150">
+        <v>71</v>
+      </c>
+      <c r="G150" t="s">
+        <v>10</v>
+      </c>
+      <c r="H150" t="s">
+        <v>10</v>
+      </c>
+      <c r="I150" t="s">
+        <v>10</v>
+      </c>
+      <c r="J150">
         <v>245</v>
       </c>
     </row>

</xml_diff>